<commit_message>
user db 생성 및 signup db 연동
</commit_message>
<xml_diff>
--- a/웹 구조 및 디비.xlsx
+++ b/웹 구조 및 디비.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyh\Desktop\국비지원 교육 자료\web1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928586C2-4BB3-4795-8085-CF19F7C26736}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FCE97D-44E7-4582-9509-DC32F527FB65}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B59F6CB1-8AF3-40DD-9BAA-E845A5CC53F8}"/>
+    <workbookView xWindow="3852" yWindow="588" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{B59F6CB1-8AF3-40DD-9BAA-E845A5CC53F8}"/>
   </bookViews>
   <sheets>
     <sheet name="웹구조" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -120,10 +120,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>생년월일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -204,14 +200,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>engname</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>call</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -221,10 +209,6 @@
   </si>
   <si>
     <t>country</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>birthday</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -296,6 +280,30 @@
   <si>
     <t>메인
 (main_app)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name_ko</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name_eng</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>성별</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sex</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생년월일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>birthday</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -413,17 +421,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -741,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3455FB84-6E84-4361-A615-150B8FA28B07}">
   <dimension ref="B3:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -754,115 +762,115 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B5" s="5"/>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B6" s="5"/>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B8" s="6"/>
+      <c r="C8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="B9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B4" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B5" s="3"/>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B6" s="3"/>
-      <c r="C6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B7" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B8" s="4"/>
-      <c r="C8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
-      <c r="B9" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -878,10 +886,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6354CE-D8C6-43E4-840C-F875131785E1}">
-  <dimension ref="B2:K8"/>
+  <dimension ref="B2:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -889,15 +897,18 @@
     <col min="2" max="2" width="10.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="12" max="12" width="9.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -926,39 +937,45 @@
         <v>19</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
         <v>41</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>45</v>
       </c>
-      <c r="H4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>48</v>
-      </c>
       <c r="K4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+        <v>68</v>
+      </c>
+      <c r="L4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -990,36 +1007,36 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" t="s">
-        <v>56</v>
-      </c>
-      <c r="K6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1030,34 +1047,35 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
디비 컬럼명 변경 및 ticket, reser, airline 디비 선언
</commit_message>
<xml_diff>
--- a/웹 구조 및 디비.xlsx
+++ b/웹 구조 및 디비.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jyh\Desktop\국비지원 교육 자료\web1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E0C492-7615-4C12-BB5D-47F9302EF547}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5640B5DB-4CC2-4C6E-931D-BB6739311D8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="672" windowWidth="17280" windowHeight="9072" activeTab="1" xr2:uid="{B59F6CB1-8AF3-40DD-9BAA-E845A5CC53F8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B59F6CB1-8AF3-40DD-9BAA-E845A5CC53F8}"/>
   </bookViews>
   <sheets>
     <sheet name="웹구조" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="84">
   <si>
     <t>테이블명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,10 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>가격</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Ticket</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -208,51 +204,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>goplace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>comeplace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>goariport</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>comeairport</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>gotime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>cometime</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>airline</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>user_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ticket_id_go</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ticket_id_come</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -340,6 +292,78 @@
   </si>
   <si>
     <t>날짜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일등석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first_class_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비즈니스석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>business_class_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>프리미엄석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>premium_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반석</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>economy_price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>go_ticket_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>come_ticket_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reservation_date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>airline_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>departure_place</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrival_place</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>departure_airport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrival_airport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>departure_time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrival_time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -798,115 +822,115 @@
   <sheetData>
     <row r="3" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B5" s="5"/>
       <c r="C5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B6" s="5"/>
       <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B7" s="4" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B8" s="6"/>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="B9" s="3" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="E9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -922,10 +946,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6354CE-D8C6-43E4-840C-F875131785E1}">
-  <dimension ref="B2:L10"/>
+  <dimension ref="B2:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -933,18 +957,22 @@
     <col min="2" max="2" width="10.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5" customWidth="1"/>
-    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.8984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -961,71 +989,71 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
       </c>
       <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
+      <c r="L3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
         <v>18</v>
       </c>
-      <c r="K3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="C4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" t="s">
-        <v>44</v>
-      </c>
-      <c r="K4" t="s">
-        <v>65</v>
-      </c>
-      <c r="L4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
       </c>
       <c r="G5" t="s">
         <v>9</v>
@@ -1040,70 +1068,88 @@
         <v>12</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="L5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="C6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="G6" t="s">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
       <c r="I6" t="s">
-        <v>50</v>
+        <v>82</v>
       </c>
       <c r="J6" t="s">
-        <v>51</v>
+        <v>83</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="L6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+      <c r="M6" t="s">
+        <v>69</v>
+      </c>
+      <c r="N6" t="s">
+        <v>71</v>
+      </c>
+      <c r="O6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.4">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -1114,30 +1160,30 @@
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.4">
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="F10" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="G10" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>